<commit_message>
Included EQUIPMENT eval, updated folder structure, allowed for multiple archive excels
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/1_rt_component_series/qoq_rt_data_DOMUSE.xlsx
+++ b/0_0_Data/2_Processed_Data/1_rt_component_series/qoq_rt_data_DOMUSE.xlsx
@@ -380,13 +380,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA83"/>
+  <dimension ref="A1:BB84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:54">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,8 +546,11 @@
       <c r="BA1" s="2">
         <v>45891</v>
       </c>
+      <c r="BB1" s="2">
+        <v>45986</v>
+      </c>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:54">
       <c r="A2" s="2">
         <v>38398</v>
       </c>
@@ -707,8 +710,11 @@
       <c r="BA2">
         <v>-1.019024872684525</v>
       </c>
+      <c r="BB2">
+        <v>-1.019024872684525</v>
+      </c>
     </row>
-    <row r="3" spans="1:53">
+    <row r="3" spans="1:54">
       <c r="A3" s="2">
         <v>38487</v>
       </c>
@@ -868,8 +874,11 @@
       <c r="BA3">
         <v>0.8876024303436765</v>
       </c>
+      <c r="BB3">
+        <v>0.8876024303436765</v>
+      </c>
     </row>
-    <row r="4" spans="1:53">
+    <row r="4" spans="1:54">
       <c r="A4" s="2">
         <v>38579</v>
       </c>
@@ -1029,8 +1038,11 @@
       <c r="BA4">
         <v>0.501281665261132</v>
       </c>
+      <c r="BB4">
+        <v>0.501281665261132</v>
+      </c>
     </row>
-    <row r="5" spans="1:53">
+    <row r="5" spans="1:54">
       <c r="A5" s="2">
         <v>38671</v>
       </c>
@@ -1190,8 +1202,11 @@
       <c r="BA5">
         <v>0.783791364788172</v>
       </c>
+      <c r="BB5">
+        <v>0.783791364788172</v>
+      </c>
     </row>
-    <row r="6" spans="1:53">
+    <row r="6" spans="1:54">
       <c r="A6" s="2">
         <v>38763</v>
       </c>
@@ -1351,8 +1366,11 @@
       <c r="BA6">
         <v>0.5095734791538149</v>
       </c>
+      <c r="BB6">
+        <v>0.5095734791538149</v>
+      </c>
     </row>
-    <row r="7" spans="1:53">
+    <row r="7" spans="1:54">
       <c r="A7" s="2">
         <v>38852</v>
       </c>
@@ -1512,8 +1530,11 @@
       <c r="BA7">
         <v>1.170187288160236</v>
       </c>
+      <c r="BB7">
+        <v>1.170187288160236</v>
+      </c>
     </row>
-    <row r="8" spans="1:53">
+    <row r="8" spans="1:54">
       <c r="A8" s="2">
         <v>38944</v>
       </c>
@@ -1673,8 +1694,11 @@
       <c r="BA8">
         <v>0.5284639015385721</v>
       </c>
+      <c r="BB8">
+        <v>0.5284639015385721</v>
+      </c>
     </row>
-    <row r="9" spans="1:53">
+    <row r="9" spans="1:54">
       <c r="A9" s="2">
         <v>39036</v>
       </c>
@@ -1834,8 +1858,11 @@
       <c r="BA9">
         <v>-0.9224347173962713</v>
       </c>
+      <c r="BB9">
+        <v>-0.9224347173962713</v>
+      </c>
     </row>
-    <row r="10" spans="1:53">
+    <row r="10" spans="1:54">
       <c r="A10" s="2">
         <v>39128</v>
       </c>
@@ -1995,8 +2022,11 @@
       <c r="BA10">
         <v>1.638479263879859</v>
       </c>
+      <c r="BB10">
+        <v>1.638479263879859</v>
+      </c>
     </row>
-    <row r="11" spans="1:53">
+    <row r="11" spans="1:54">
       <c r="A11" s="2">
         <v>39217</v>
       </c>
@@ -2156,8 +2186,11 @@
       <c r="BA11">
         <v>-0.8367887460914147</v>
       </c>
+      <c r="BB11">
+        <v>-0.8367887460914147</v>
+      </c>
     </row>
-    <row r="12" spans="1:53">
+    <row r="12" spans="1:54">
       <c r="A12" s="2">
         <v>39309</v>
       </c>
@@ -2317,8 +2350,11 @@
       <c r="BA12">
         <v>0.9530509214829834</v>
       </c>
+      <c r="BB12">
+        <v>0.9530509214829834</v>
+      </c>
     </row>
-    <row r="13" spans="1:53">
+    <row r="13" spans="1:54">
       <c r="A13" s="2">
         <v>39401</v>
       </c>
@@ -2475,8 +2511,11 @@
       <c r="BA13">
         <v>-0.6785311155745859</v>
       </c>
+      <c r="BB13">
+        <v>-0.6785311155745859</v>
+      </c>
     </row>
-    <row r="14" spans="1:53">
+    <row r="14" spans="1:54">
       <c r="A14" s="2">
         <v>39493</v>
       </c>
@@ -2633,8 +2672,11 @@
       <c r="BA14">
         <v>1.602887836530243</v>
       </c>
+      <c r="BB14">
+        <v>1.602887836530243</v>
+      </c>
     </row>
-    <row r="15" spans="1:53">
+    <row r="15" spans="1:54">
       <c r="A15" s="2">
         <v>39583</v>
       </c>
@@ -2788,8 +2830,11 @@
       <c r="BA15">
         <v>-1.258229598656428</v>
       </c>
+      <c r="BB15">
+        <v>-1.258229598656428</v>
+      </c>
     </row>
-    <row r="16" spans="1:53">
+    <row r="16" spans="1:54">
       <c r="A16" s="2">
         <v>39675</v>
       </c>
@@ -2943,8 +2988,11 @@
       <c r="BA16">
         <v>0.7939633611163259</v>
       </c>
+      <c r="BB16">
+        <v>0.7939633611163259</v>
+      </c>
     </row>
-    <row r="17" spans="1:53">
+    <row r="17" spans="1:54">
       <c r="A17" s="2">
         <v>39767</v>
       </c>
@@ -3095,8 +3143,11 @@
       <c r="BA17">
         <v>-0.5251394922476749</v>
       </c>
+      <c r="BB17">
+        <v>-0.5251394922476749</v>
+      </c>
     </row>
-    <row r="18" spans="1:53">
+    <row r="18" spans="1:54">
       <c r="A18" s="2">
         <v>39859</v>
       </c>
@@ -3247,8 +3298,11 @@
       <c r="BA18">
         <v>-1.32903296106565</v>
       </c>
+      <c r="BB18">
+        <v>-1.32903296106565</v>
+      </c>
     </row>
-    <row r="19" spans="1:53">
+    <row r="19" spans="1:54">
       <c r="A19" s="2">
         <v>39948</v>
       </c>
@@ -3396,8 +3450,11 @@
       <c r="BA19">
         <v>-1.501005349787889</v>
       </c>
+      <c r="BB19">
+        <v>-1.501005349787889</v>
+      </c>
     </row>
-    <row r="20" spans="1:53">
+    <row r="20" spans="1:54">
       <c r="A20" s="2">
         <v>40040</v>
       </c>
@@ -3545,8 +3602,11 @@
       <c r="BA20">
         <v>1.094075326722859</v>
       </c>
+      <c r="BB20">
+        <v>1.094075326722859</v>
+      </c>
     </row>
-    <row r="21" spans="1:53">
+    <row r="21" spans="1:54">
       <c r="A21" s="2">
         <v>40132</v>
       </c>
@@ -3691,8 +3751,11 @@
       <c r="BA21">
         <v>-0.6087605469991217</v>
       </c>
+      <c r="BB21">
+        <v>-0.6087605469991217</v>
+      </c>
     </row>
-    <row r="22" spans="1:53">
+    <row r="22" spans="1:54">
       <c r="A22" s="2">
         <v>40224</v>
       </c>
@@ -3837,8 +3900,11 @@
       <c r="BA22">
         <v>1.636155096406839</v>
       </c>
+      <c r="BB22">
+        <v>1.636155096406839</v>
+      </c>
     </row>
-    <row r="23" spans="1:53">
+    <row r="23" spans="1:54">
       <c r="A23" s="2">
         <v>40313</v>
       </c>
@@ -3980,8 +4046,11 @@
       <c r="BA23">
         <v>1.53095784658872</v>
       </c>
+      <c r="BB23">
+        <v>1.53095784658872</v>
+      </c>
     </row>
-    <row r="24" spans="1:53">
+    <row r="24" spans="1:54">
       <c r="A24" s="2">
         <v>40405</v>
       </c>
@@ -4123,8 +4192,11 @@
       <c r="BA24">
         <v>0.1790633318223627</v>
       </c>
+      <c r="BB24">
+        <v>0.1790633318223627</v>
+      </c>
     </row>
-    <row r="25" spans="1:53">
+    <row r="25" spans="1:54">
       <c r="A25" s="2">
         <v>40497</v>
       </c>
@@ -4263,8 +4335,11 @@
       <c r="BA25">
         <v>0.3480705421442281</v>
       </c>
+      <c r="BB25">
+        <v>0.3480705421442281</v>
+      </c>
     </row>
-    <row r="26" spans="1:53">
+    <row r="26" spans="1:54">
       <c r="A26" s="2">
         <v>40589</v>
       </c>
@@ -4403,8 +4478,11 @@
       <c r="BA26">
         <v>1.451221515208928</v>
       </c>
+      <c r="BB26">
+        <v>1.451221515208928</v>
+      </c>
     </row>
-    <row r="27" spans="1:53">
+    <row r="27" spans="1:54">
       <c r="A27" s="2">
         <v>40678</v>
       </c>
@@ -4540,8 +4618,11 @@
       <c r="BA27">
         <v>0.8239934654972245</v>
       </c>
+      <c r="BB27">
+        <v>0.8239934654972245</v>
+      </c>
     </row>
-    <row r="28" spans="1:53">
+    <row r="28" spans="1:54">
       <c r="A28" s="2">
         <v>40770</v>
       </c>
@@ -4677,8 +4758,11 @@
       <c r="BA28">
         <v>0.2020273747754828</v>
       </c>
+      <c r="BB28">
+        <v>0.2020273747754828</v>
+      </c>
     </row>
-    <row r="29" spans="1:53">
+    <row r="29" spans="1:54">
       <c r="A29" s="2">
         <v>40862</v>
       </c>
@@ -4811,8 +4895,11 @@
       <c r="BA29">
         <v>0.03665234221521985</v>
       </c>
+      <c r="BB29">
+        <v>0.03665234221521985</v>
+      </c>
     </row>
-    <row r="30" spans="1:53">
+    <row r="30" spans="1:54">
       <c r="A30" s="2">
         <v>40954</v>
       </c>
@@ -4945,8 +5032,11 @@
       <c r="BA30">
         <v>-0.3568640125838272</v>
       </c>
+      <c r="BB30">
+        <v>-0.3568640125838272</v>
+      </c>
     </row>
-    <row r="31" spans="1:53">
+    <row r="31" spans="1:54">
       <c r="A31" s="2">
         <v>41044</v>
       </c>
@@ -5076,8 +5166,11 @@
       <c r="BA31">
         <v>-0.6140442841884663</v>
       </c>
+      <c r="BB31">
+        <v>-0.6140442841884663</v>
+      </c>
     </row>
-    <row r="32" spans="1:53">
+    <row r="32" spans="1:54">
       <c r="A32" s="2">
         <v>41136</v>
       </c>
@@ -5207,8 +5300,11 @@
       <c r="BA32">
         <v>-0.4707272781813003</v>
       </c>
+      <c r="BB32">
+        <v>-0.4707272781813003</v>
+      </c>
     </row>
-    <row r="33" spans="1:53">
+    <row r="33" spans="1:54">
       <c r="A33" s="2">
         <v>41228</v>
       </c>
@@ -5335,8 +5431,11 @@
       <c r="BA33">
         <v>0.6798763458711505</v>
       </c>
+      <c r="BB33">
+        <v>0.6798763458711505</v>
+      </c>
     </row>
-    <row r="34" spans="1:53">
+    <row r="34" spans="1:54">
       <c r="A34" s="2">
         <v>41320</v>
       </c>
@@ -5463,8 +5562,11 @@
       <c r="BA34">
         <v>-0.4549252105260422</v>
       </c>
+      <c r="BB34">
+        <v>-0.4549252105260422</v>
+      </c>
     </row>
-    <row r="35" spans="1:53">
+    <row r="35" spans="1:54">
       <c r="A35" s="2">
         <v>41409</v>
       </c>
@@ -5588,8 +5690,11 @@
       <c r="BA35">
         <v>0.8156466047582853</v>
       </c>
+      <c r="BB35">
+        <v>0.8156466047582853</v>
+      </c>
     </row>
-    <row r="36" spans="1:53">
+    <row r="36" spans="1:54">
       <c r="A36" s="2">
         <v>41501</v>
       </c>
@@ -5713,8 +5818,11 @@
       <c r="BA36">
         <v>0.9357631895998964</v>
       </c>
+      <c r="BB36">
+        <v>0.9357631895998964</v>
+      </c>
     </row>
-    <row r="37" spans="1:53">
+    <row r="37" spans="1:54">
       <c r="A37" s="2">
         <v>41593</v>
       </c>
@@ -5835,8 +5943,11 @@
       <c r="BA37">
         <v>-0.1255439525040316</v>
       </c>
+      <c r="BB37">
+        <v>-0.1255439525040316</v>
+      </c>
     </row>
-    <row r="38" spans="1:53">
+    <row r="38" spans="1:54">
       <c r="A38" s="2">
         <v>41685</v>
       </c>
@@ -5957,8 +6068,11 @@
       <c r="BA38">
         <v>0.8309616106594575</v>
       </c>
+      <c r="BB38">
+        <v>0.8309616106594575</v>
+      </c>
     </row>
-    <row r="39" spans="1:53">
+    <row r="39" spans="1:54">
       <c r="A39" s="2">
         <v>41774</v>
       </c>
@@ -6076,8 +6190,11 @@
       <c r="BA39">
         <v>0.13455620655985</v>
       </c>
+      <c r="BB39">
+        <v>0.13455620655985</v>
+      </c>
     </row>
-    <row r="40" spans="1:53">
+    <row r="40" spans="1:54">
       <c r="A40" s="2">
         <v>41866</v>
       </c>
@@ -6195,8 +6312,11 @@
       <c r="BA40">
         <v>-0.3839223037353605</v>
       </c>
+      <c r="BB40">
+        <v>-0.3839223037353605</v>
+      </c>
     </row>
-    <row r="41" spans="1:53">
+    <row r="41" spans="1:54">
       <c r="A41" s="2">
         <v>41958</v>
       </c>
@@ -6311,8 +6431,11 @@
       <c r="BA41">
         <v>0.8864082508326874</v>
       </c>
+      <c r="BB41">
+        <v>0.8864082508326874</v>
+      </c>
     </row>
-    <row r="42" spans="1:53">
+    <row r="42" spans="1:54">
       <c r="A42" s="2">
         <v>42050</v>
       </c>
@@ -6427,8 +6550,11 @@
       <c r="BA42">
         <v>0.2947380355466294</v>
       </c>
+      <c r="BB42">
+        <v>0.2947380355466294</v>
+      </c>
     </row>
-    <row r="43" spans="1:53">
+    <row r="43" spans="1:54">
       <c r="A43" s="2">
         <v>42139</v>
       </c>
@@ -6540,8 +6666,11 @@
       <c r="BA43">
         <v>-0.07583325464557333</v>
       </c>
+      <c r="BB43">
+        <v>-0.07583325464557333</v>
+      </c>
     </row>
-    <row r="44" spans="1:53">
+    <row r="44" spans="1:54">
       <c r="A44" s="2">
         <v>42231</v>
       </c>
@@ -6653,8 +6782,11 @@
       <c r="BA44">
         <v>0.7873983253725783</v>
       </c>
+      <c r="BB44">
+        <v>0.7873983253725783</v>
+      </c>
     </row>
-    <row r="45" spans="1:53">
+    <row r="45" spans="1:54">
       <c r="A45" s="2">
         <v>42323</v>
       </c>
@@ -6763,8 +6895,11 @@
       <c r="BA45">
         <v>0.9695092796512768</v>
       </c>
+      <c r="BB45">
+        <v>0.9695092796512768</v>
+      </c>
     </row>
-    <row r="46" spans="1:53">
+    <row r="46" spans="1:54">
       <c r="A46" s="2">
         <v>42415</v>
       </c>
@@ -6873,8 +7008,11 @@
       <c r="BA46">
         <v>0.6245863217464631</v>
       </c>
+      <c r="BB46">
+        <v>0.6245863217464631</v>
+      </c>
     </row>
-    <row r="47" spans="1:53">
+    <row r="47" spans="1:54">
       <c r="A47" s="2">
         <v>42505</v>
       </c>
@@ -6980,8 +7118,11 @@
       <c r="BA47">
         <v>0.04631981473890789</v>
       </c>
+      <c r="BB47">
+        <v>0.04631981473890789</v>
+      </c>
     </row>
-    <row r="48" spans="1:53">
+    <row r="48" spans="1:54">
       <c r="A48" s="2">
         <v>42597</v>
       </c>
@@ -7087,8 +7228,11 @@
       <c r="BA48">
         <v>0.5741282506780578</v>
       </c>
+      <c r="BB48">
+        <v>0.5741282506780578</v>
+      </c>
     </row>
-    <row r="49" spans="1:53">
+    <row r="49" spans="1:54">
       <c r="A49" s="2">
         <v>42689</v>
       </c>
@@ -7191,8 +7335,11 @@
       <c r="BA49">
         <v>0.6629265129002277</v>
       </c>
+      <c r="BB49">
+        <v>0.6629265129002277</v>
+      </c>
     </row>
-    <row r="50" spans="1:53">
+    <row r="50" spans="1:54">
       <c r="A50" s="2">
         <v>42781</v>
       </c>
@@ -7295,8 +7442,11 @@
       <c r="BA50">
         <v>0.3877663769499975</v>
       </c>
+      <c r="BB50">
+        <v>0.3877663769499975</v>
+      </c>
     </row>
-    <row r="51" spans="1:53">
+    <row r="51" spans="1:54">
       <c r="A51" s="2">
         <v>42870</v>
       </c>
@@ -7396,8 +7546,11 @@
       <c r="BA51">
         <v>1.117874141853932</v>
       </c>
+      <c r="BB51">
+        <v>1.117874141853932</v>
+      </c>
     </row>
-    <row r="52" spans="1:53">
+    <row r="52" spans="1:54">
       <c r="A52" s="2">
         <v>42962</v>
       </c>
@@ -7497,8 +7650,11 @@
       <c r="BA52">
         <v>0.359515012501916</v>
       </c>
+      <c r="BB52">
+        <v>0.359515012501916</v>
+      </c>
     </row>
-    <row r="53" spans="1:53">
+    <row r="53" spans="1:54">
       <c r="A53" s="2">
         <v>43054</v>
       </c>
@@ -7595,8 +7751,11 @@
       <c r="BA53">
         <v>0.1242992151364578</v>
       </c>
+      <c r="BB53">
+        <v>0.1242992151364578</v>
+      </c>
     </row>
-    <row r="54" spans="1:53">
+    <row r="54" spans="1:54">
       <c r="A54" s="2">
         <v>43146</v>
       </c>
@@ -7690,8 +7849,11 @@
       <c r="BA54">
         <v>0.1571952554336775</v>
       </c>
+      <c r="BB54">
+        <v>0.1571952554336775</v>
+      </c>
     </row>
-    <row r="55" spans="1:53">
+    <row r="55" spans="1:54">
       <c r="A55" s="2">
         <v>43235</v>
       </c>
@@ -7782,8 +7944,11 @@
       <c r="BA55">
         <v>0.7965518134806615</v>
       </c>
+      <c r="BB55">
+        <v>0.7965518134806615</v>
+      </c>
     </row>
-    <row r="56" spans="1:53">
+    <row r="56" spans="1:54">
       <c r="A56" s="2">
         <v>43327</v>
       </c>
@@ -7871,8 +8036,11 @@
       <c r="BA56">
         <v>0.6786821427891851</v>
       </c>
+      <c r="BB56">
+        <v>0.6786821427891851</v>
+      </c>
     </row>
-    <row r="57" spans="1:53">
+    <row r="57" spans="1:54">
       <c r="A57" s="2">
         <v>43419</v>
       </c>
@@ -7957,8 +8125,11 @@
       <c r="BA57">
         <v>0.424793870183592</v>
       </c>
+      <c r="BB57">
+        <v>0.424793870183592</v>
+      </c>
     </row>
-    <row r="58" spans="1:53">
+    <row r="58" spans="1:54">
       <c r="A58" s="2">
         <v>43511</v>
       </c>
@@ -8040,8 +8211,11 @@
       <c r="BA58">
         <v>0.3</v>
       </c>
+      <c r="BB58">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="59" spans="1:53">
+    <row r="59" spans="1:54">
       <c r="A59" s="2">
         <v>43600</v>
       </c>
@@ -8120,8 +8294,11 @@
       <c r="BA59">
         <v>0.3</v>
       </c>
+      <c r="BB59">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="60" spans="1:53">
+    <row r="60" spans="1:54">
       <c r="A60" s="2">
         <v>43692</v>
       </c>
@@ -8197,8 +8374,11 @@
       <c r="BA60">
         <v>-0.5</v>
       </c>
+      <c r="BB60">
+        <v>-0.5</v>
+      </c>
     </row>
-    <row r="61" spans="1:53">
+    <row r="61" spans="1:54">
       <c r="A61" s="2">
         <v>43784</v>
       </c>
@@ -8271,8 +8451,11 @@
       <c r="BA61">
         <v>0.3</v>
       </c>
+      <c r="BB61">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="62" spans="1:53">
+    <row r="62" spans="1:54">
       <c r="A62" s="2">
         <v>43876</v>
       </c>
@@ -8342,8 +8525,11 @@
       <c r="BA62">
         <v>-0.9728763394718669</v>
       </c>
+      <c r="BB62">
+        <v>-0.9728763394718669</v>
+      </c>
     </row>
-    <row r="63" spans="1:53">
+    <row r="63" spans="1:54">
       <c r="A63" s="2">
         <v>43966</v>
       </c>
@@ -8410,8 +8596,11 @@
       <c r="BA63">
         <v>-7.646786505763302</v>
       </c>
+      <c r="BB63">
+        <v>-7.646786505763302</v>
+      </c>
     </row>
-    <row r="64" spans="1:53">
+    <row r="64" spans="1:54">
       <c r="A64" s="2">
         <v>44058</v>
       </c>
@@ -8475,8 +8664,11 @@
       <c r="BA64">
         <v>5.056075122789721</v>
       </c>
+      <c r="BB64">
+        <v>5.056075122789721</v>
+      </c>
     </row>
-    <row r="65" spans="1:53">
+    <row r="65" spans="1:54">
       <c r="A65" s="2">
         <v>44150</v>
       </c>
@@ -8537,8 +8729,11 @@
       <c r="BA65">
         <v>-0.1620152258813761</v>
       </c>
+      <c r="BB65">
+        <v>-0.1620152258813761</v>
+      </c>
     </row>
-    <row r="66" spans="1:53">
+    <row r="66" spans="1:54">
       <c r="A66" s="2">
         <v>44242</v>
       </c>
@@ -8596,8 +8791,11 @@
       <c r="BA66">
         <v>-0.8490652932627256</v>
       </c>
+      <c r="BB66">
+        <v>-0.8490652932627256</v>
+      </c>
     </row>
-    <row r="67" spans="1:53">
+    <row r="67" spans="1:54">
       <c r="A67" s="2">
         <v>44331</v>
       </c>
@@ -8652,8 +8850,11 @@
       <c r="BA67">
         <v>2.57367793996282</v>
       </c>
+      <c r="BB67">
+        <v>2.57367793996282</v>
+      </c>
     </row>
-    <row r="68" spans="1:53">
+    <row r="68" spans="1:54">
       <c r="A68" s="2">
         <v>44423</v>
       </c>
@@ -8705,8 +8906,11 @@
       <c r="BA68">
         <v>1.893477998435444</v>
       </c>
+      <c r="BB68">
+        <v>1.893477998435444</v>
+      </c>
     </row>
-    <row r="69" spans="1:53">
+    <row r="69" spans="1:54">
       <c r="A69" s="2">
         <v>44515</v>
       </c>
@@ -8755,8 +8959,11 @@
       <c r="BA69">
         <v>-0.4760149577203094</v>
       </c>
+      <c r="BB69">
+        <v>-0.4760149577203094</v>
+      </c>
     </row>
-    <row r="70" spans="1:53">
+    <row r="70" spans="1:54">
       <c r="A70" s="2">
         <v>44607</v>
       </c>
@@ -8802,8 +9009,11 @@
       <c r="BA70">
         <v>1.115155785188662</v>
       </c>
+      <c r="BB70">
+        <v>1.115155785188662</v>
+      </c>
     </row>
-    <row r="71" spans="1:53">
+    <row r="71" spans="1:54">
       <c r="A71" s="2">
         <v>44696</v>
       </c>
@@ -8846,8 +9056,11 @@
       <c r="BA71">
         <v>0.5952357910519908</v>
       </c>
+      <c r="BB71">
+        <v>0.5952357910519908</v>
+      </c>
     </row>
-    <row r="72" spans="1:53">
+    <row r="72" spans="1:54">
       <c r="A72" s="2">
         <v>44788</v>
       </c>
@@ -8887,8 +9100,11 @@
       <c r="BA72">
         <v>0.8967419189327899</v>
       </c>
+      <c r="BB72">
+        <v>0.8967419189327899</v>
+      </c>
     </row>
-    <row r="73" spans="1:53">
+    <row r="73" spans="1:54">
       <c r="A73" s="2">
         <v>44880</v>
       </c>
@@ -8925,8 +9141,11 @@
       <c r="BA73">
         <v>-1.030904243755657</v>
       </c>
+      <c r="BB73">
+        <v>-1.030904243755657</v>
+      </c>
     </row>
-    <row r="74" spans="1:53">
+    <row r="74" spans="1:54">
       <c r="A74" s="2">
         <v>44972</v>
       </c>
@@ -8960,8 +9179,11 @@
       <c r="BA74">
         <v>-0.5254260915594955</v>
       </c>
+      <c r="BB74">
+        <v>-0.5254260915594955</v>
+      </c>
     </row>
-    <row r="75" spans="1:53">
+    <row r="75" spans="1:54">
       <c r="A75" s="2">
         <v>45061</v>
       </c>
@@ -8992,8 +9214,11 @@
       <c r="BA75">
         <v>0.3702002717572981</v>
       </c>
+      <c r="BB75">
+        <v>0.3702002717572981</v>
+      </c>
     </row>
-    <row r="76" spans="1:53">
+    <row r="76" spans="1:54">
       <c r="A76" s="2">
         <v>45153</v>
       </c>
@@ -9021,8 +9246,11 @@
       <c r="BA76">
         <v>-0.2788735881504181</v>
       </c>
+      <c r="BB76">
+        <v>-0.2788735881504181</v>
+      </c>
     </row>
-    <row r="77" spans="1:53">
+    <row r="77" spans="1:54">
       <c r="A77" s="2">
         <v>45245</v>
       </c>
@@ -9047,8 +9275,11 @@
       <c r="BA77">
         <v>-0.8389720173227175</v>
       </c>
+      <c r="BB77">
+        <v>-0.8389720173227175</v>
+      </c>
     </row>
-    <row r="78" spans="1:53">
+    <row r="78" spans="1:54">
       <c r="A78" s="2">
         <v>45337</v>
       </c>
@@ -9070,8 +9301,11 @@
       <c r="BA78">
         <v>0.1503986163346127</v>
       </c>
+      <c r="BB78">
+        <v>0.1503986163346127</v>
+      </c>
     </row>
-    <row r="79" spans="1:53">
+    <row r="79" spans="1:54">
       <c r="A79" s="2">
         <v>45427</v>
       </c>
@@ -9090,8 +9324,11 @@
       <c r="BA79">
         <v>-0.01906297584814354</v>
       </c>
+      <c r="BB79">
+        <v>-0.01906297584814354</v>
+      </c>
     </row>
-    <row r="80" spans="1:53">
+    <row r="80" spans="1:54">
       <c r="A80" s="2">
         <v>45519</v>
       </c>
@@ -9107,8 +9344,11 @@
       <c r="BA80">
         <v>1.268119412418997</v>
       </c>
+      <c r="BB80">
+        <v>1.268119412418997</v>
+      </c>
     </row>
-    <row r="81" spans="1:53">
+    <row r="81" spans="1:54">
       <c r="A81" s="2">
         <v>45611</v>
       </c>
@@ -9121,8 +9361,11 @@
       <c r="BA81">
         <v>0.8944503735891658</v>
       </c>
+      <c r="BB81">
+        <v>0.8944503735891658</v>
+      </c>
     </row>
-    <row r="82" spans="1:53">
+    <row r="82" spans="1:54">
       <c r="A82" s="2">
         <v>45703</v>
       </c>
@@ -9132,13 +9375,27 @@
       <c r="BA82">
         <v>-0.1212118887798113</v>
       </c>
+      <c r="BB82">
+        <v>-0.1118837721692358</v>
+      </c>
     </row>
-    <row r="83" spans="1:53">
+    <row r="83" spans="1:54">
       <c r="A83" s="2">
         <v>45792</v>
       </c>
       <c r="BA83">
         <v>0.4200898674779694</v>
+      </c>
+      <c r="BB83">
+        <v>0.3266766184601977</v>
+      </c>
+    </row>
+    <row r="84" spans="1:54">
+      <c r="A84" s="2">
+        <v>45884</v>
+      </c>
+      <c r="BB84">
+        <v>0.325608361860148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>